<commit_message>
Team Info & Roles Updated
</commit_message>
<xml_diff>
--- a/Obstacle Course Time.xlsx
+++ b/Obstacle Course Time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanzhiliu/Desktop/MHS/Science Club 2023-2024/SeaPerch 2023-2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60D40F8-B657-2747-8DEF-1B3862CA9604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807F64ED-BD5E-6446-9B13-FCF40DE9AAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{0D551839-E2EE-2540-8398-B27D1158119B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{0D551839-E2EE-2540-8398-B27D1158119B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Driver</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,10 +51,6 @@
   </si>
   <si>
     <t>Eli</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jeffrey</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -431,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2FB6FE-F4FC-AA4F-8D9B-84F3A3030C21}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -452,11 +448,8 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -470,38 +463,47 @@
         <v>8.6805555555555566E-2</v>
       </c>
       <c r="D2" s="1">
-        <v>7.3611111111111113E-2</v>
+        <v>3.9583333333333331E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>45169</v>
-      </c>
-      <c r="D3" s="1">
-        <v>3.9583333333333331E-2</v>
+        <v>45178</v>
+      </c>
+      <c r="C3" s="1">
+        <v>8.5416666666666655E-2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>45178</v>
-      </c>
-      <c r="C4" s="1">
-        <v>8.5416666666666655E-2</v>
+        <v>45183</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.15833333333333333</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>45183</v>
+        <v>45190</v>
       </c>
       <c r="B5" s="1">
-        <v>0.15833333333333333</v>
-      </c>
-      <c r="F5" t="s">
-        <v>6</v>
-      </c>
+        <v>0.14444444444444446</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>8.1944444444444445E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D6" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>